<commit_message>
modified:   ExPECA-HW-Discovery.xlsx 	modified:   excel-to-md.py 	modified:   inventory.md
</commit_message>
<xml_diff>
--- a/ExPECA-HW-Discovery.xlsx
+++ b/ExPECA-HW-Discovery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssmos/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ug.kth.se\dfs\home\s\t\steron\appdata\xp.V2\Documents\expeca\lab-inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B66A220-E990-0545-A4A3-890A55C692B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161374DA-6AE5-4D2E-936D-9D25E1890C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Telenor Network" sheetId="12" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="891">
   <si>
     <t>Dell PowerEdge R750xs</t>
   </si>
@@ -2651,13 +2651,67 @@
   </si>
   <si>
     <t>999080000000005</t>
+  </si>
+  <si>
+    <t>worker-21</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4</t>
+  </si>
+  <si>
+    <t>Broadcom BCM2711 @ 1.5 GHz</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>8 GB</t>
+  </si>
+  <si>
+    <t>64 GB microSD</t>
+  </si>
+  <si>
+    <t>te1/0/25</t>
+  </si>
+  <si>
+    <t>dc:a6:32:bf:52:b0</t>
+  </si>
+  <si>
+    <t>Broadcom GENET (BCM54213) 1-port Gigabit Ethernet</t>
+  </si>
+  <si>
+    <t>enx000acd47c9fc</t>
+  </si>
+  <si>
+    <t>enx000acd47cdaf</t>
+  </si>
+  <si>
+    <t>enx000acd47cdb0</t>
+  </si>
+  <si>
+    <t>00:0a:cd:47:c9:fc</t>
+  </si>
+  <si>
+    <t>00:0a:cd:47:cd:af</t>
+  </si>
+  <si>
+    <t>00:0a:cd:47:cd:b0</t>
+  </si>
+  <si>
+    <t>te3/0/5</t>
+  </si>
+  <si>
+    <t>te4/0/4</t>
+  </si>
+  <si>
+    <t>ASIX AX88179 (StarTech USB32000SPT) 1-port Gigabit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3228,20 +3282,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="25.5" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
-    <col min="12" max="12" width="61.33203125" customWidth="1"/>
+    <col min="1" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3258,7 +3312,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>468</v>
       </c>
@@ -3275,7 +3329,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -3313,7 +3367,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>272</v>
       </c>
@@ -3365,21 +3419,21 @@
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="25.5" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
-    <col min="12" max="12" width="61.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3396,7 +3450,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="3" t="s">
         <v>464</v>
       </c>
@@ -3413,7 +3467,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -3451,7 +3505,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>471</v>
       </c>
@@ -3503,21 +3557,21 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="25.5" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
-    <col min="12" max="12" width="61.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3532,7 +3586,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="3" t="s">
         <v>460</v>
       </c>
@@ -3547,7 +3601,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -3585,7 +3639,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>242</v>
       </c>
@@ -3623,7 +3677,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
         <v>243</v>
       </c>
@@ -3671,25 +3725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DF0E2B-725B-3247-9FD1-11D5F10AA821}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="106" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="25.5" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
-    <col min="12" max="12" width="61.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="25.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3712,7 +3766,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>231</v>
       </c>
@@ -3735,7 +3789,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -3773,7 +3827,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="s">
         <v>242</v>
       </c>
@@ -3811,7 +3865,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
         <v>243</v>
       </c>
@@ -3849,7 +3903,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" s="4" t="s">
         <v>244</v>
       </c>
@@ -3887,7 +3941,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3910,7 +3964,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>252</v>
       </c>
@@ -3933,7 +3987,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>241</v>
       </c>
@@ -3971,7 +4025,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" s="4" t="s">
         <v>242</v>
       </c>
@@ -4009,7 +4063,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="4" t="s">
         <v>243</v>
       </c>
@@ -4047,7 +4101,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="4" t="s">
         <v>244</v>
       </c>
@@ -4085,10 +4139,10 @@
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="16.5">
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -4111,7 +4165,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="3" t="s">
         <v>253</v>
       </c>
@@ -4134,7 +4188,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>241</v>
       </c>
@@ -4172,7 +4226,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="4" t="s">
         <v>242</v>
       </c>
@@ -4210,7 +4264,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="4" t="s">
         <v>243</v>
       </c>
@@ -4248,7 +4302,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="30">
       <c r="A27" s="4" t="s">
         <v>244</v>
       </c>
@@ -4286,7 +4340,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -4314,7 +4368,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="9" t="s">
         <v>254</v>
       </c>
@@ -4340,7 +4394,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -4354,7 +4408,7 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="6" t="s">
         <v>241</v>
       </c>
@@ -4392,7 +4446,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="30">
       <c r="A35" s="4" t="s">
         <v>242</v>
       </c>
@@ -4430,7 +4484,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="4" t="s">
         <v>243</v>
       </c>
@@ -4468,7 +4522,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="4" t="s">
         <v>244</v>
       </c>
@@ -4506,7 +4560,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="6" t="s">
         <v>10</v>
       </c>
@@ -4532,7 +4586,7 @@
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="9" t="s">
         <v>255</v>
       </c>
@@ -4560,7 +4614,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -4574,7 +4628,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" s="6" t="s">
         <v>241</v>
       </c>
@@ -4612,7 +4666,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="30">
       <c r="A45" s="4" t="s">
         <v>242</v>
       </c>
@@ -4650,7 +4704,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="4" t="s">
         <v>243</v>
       </c>
@@ -4688,7 +4742,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="30">
       <c r="A47" s="4" t="s">
         <v>244</v>
       </c>
@@ -4726,7 +4780,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" s="6" t="s">
         <v>10</v>
       </c>
@@ -4752,7 +4806,7 @@
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="A52" s="9" t="s">
         <v>256</v>
       </c>
@@ -4780,7 +4834,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -4794,7 +4848,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
     </row>
-    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="A54" s="6" t="s">
         <v>241</v>
       </c>
@@ -4832,7 +4886,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="30">
       <c r="A55" s="4" t="s">
         <v>242</v>
       </c>
@@ -4870,7 +4924,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" s="4" t="s">
         <v>243</v>
       </c>
@@ -4908,7 +4962,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="30">
       <c r="A57" s="4" t="s">
         <v>244</v>
       </c>
@@ -4946,7 +5000,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12">
       <c r="A61" s="6" t="s">
         <v>10</v>
       </c>
@@ -4972,7 +5026,7 @@
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
     </row>
-    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12">
       <c r="A62" s="9" t="s">
         <v>257</v>
       </c>
@@ -5000,7 +5054,7 @@
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12">
       <c r="A63" s="12"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -5014,7 +5068,7 @@
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
     </row>
-    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12">
       <c r="A64" s="6" t="s">
         <v>241</v>
       </c>
@@ -5052,7 +5106,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="30">
       <c r="A65" s="4" t="s">
         <v>242</v>
       </c>
@@ -5090,7 +5144,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12">
       <c r="A66" s="4" t="s">
         <v>243</v>
       </c>
@@ -5128,7 +5182,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="30">
       <c r="A67" s="4" t="s">
         <v>244</v>
       </c>
@@ -5166,7 +5220,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12">
       <c r="A71" s="6" t="s">
         <v>10</v>
       </c>
@@ -5192,7 +5246,7 @@
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
     </row>
-    <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12">
       <c r="A72" s="9" t="s">
         <v>258</v>
       </c>
@@ -5218,7 +5272,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12">
       <c r="A73" s="12"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
@@ -5232,7 +5286,7 @@
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
     </row>
-    <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12">
       <c r="A74" s="6" t="s">
         <v>241</v>
       </c>
@@ -5270,7 +5324,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="30">
       <c r="A75" s="4" t="s">
         <v>242</v>
       </c>
@@ -5308,7 +5362,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12">
       <c r="A76" s="4" t="s">
         <v>243</v>
       </c>
@@ -5346,7 +5400,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="30">
       <c r="A77" s="4" t="s">
         <v>244</v>
       </c>
@@ -5384,7 +5438,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12">
       <c r="A81" s="6" t="s">
         <v>10</v>
       </c>
@@ -5410,7 +5464,7 @@
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
     </row>
-    <row r="82" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12">
       <c r="A82" s="9" t="s">
         <v>259</v>
       </c>
@@ -5438,7 +5492,7 @@
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12">
       <c r="A83" s="12"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -5452,7 +5506,7 @@
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
     </row>
-    <row r="84" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12">
       <c r="A84" s="6" t="s">
         <v>241</v>
       </c>
@@ -5490,7 +5544,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="30">
       <c r="A85" s="4" t="s">
         <v>242</v>
       </c>
@@ -5528,7 +5582,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12">
       <c r="A86" s="4" t="s">
         <v>243</v>
       </c>
@@ -5566,7 +5620,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="30">
       <c r="A87" s="4" t="s">
         <v>244</v>
       </c>
@@ -5604,7 +5658,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12">
       <c r="A91" s="6" t="s">
         <v>10</v>
       </c>
@@ -5630,7 +5684,7 @@
       <c r="K91" s="8"/>
       <c r="L91" s="8"/>
     </row>
-    <row r="92" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12">
       <c r="A92" s="9" t="s">
         <v>260</v>
       </c>
@@ -5656,7 +5710,7 @@
       <c r="K92" s="8"/>
       <c r="L92" s="8"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12">
       <c r="A93" s="12"/>
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
@@ -5670,7 +5724,7 @@
       <c r="K93" s="8"/>
       <c r="L93" s="8"/>
     </row>
-    <row r="94" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12">
       <c r="A94" s="6" t="s">
         <v>241</v>
       </c>
@@ -5708,7 +5762,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="30">
       <c r="A95" s="4" t="s">
         <v>242</v>
       </c>
@@ -5746,7 +5800,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12">
       <c r="A96" s="4" t="s">
         <v>243</v>
       </c>
@@ -5784,7 +5838,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="30">
       <c r="A97" s="4" t="s">
         <v>244</v>
       </c>
@@ -5836,18 +5890,18 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="26" style="19" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="11.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.33203125" style="19" customWidth="1"/>
-    <col min="12" max="12" width="43.1640625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="19"/>
+    <col min="5" max="5" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.28515625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="43.140625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.85546875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="18.75">
       <c r="A1" s="22" t="s">
         <v>840</v>
       </c>
@@ -5917,7 +5971,7 @@
       <c r="W1" s="21"/>
       <c r="X1" s="21"/>
     </row>
-    <row r="2" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="112.5">
       <c r="A2" s="23" t="s">
         <v>852</v>
       </c>
@@ -5987,7 +6041,7 @@
       <c r="W2" s="21"/>
       <c r="X2" s="21"/>
     </row>
-    <row r="3" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="112.5">
       <c r="A3" s="23" t="s">
         <v>851</v>
       </c>
@@ -6057,7 +6111,7 @@
       <c r="W3" s="21"/>
       <c r="X3" s="21"/>
     </row>
-    <row r="4" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="112.5">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -6121,7 +6175,7 @@
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
     </row>
-    <row r="5" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="112.5">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -6185,7 +6239,7 @@
       <c r="W5" s="21"/>
       <c r="X5" s="21"/>
     </row>
-    <row r="6" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="112.5">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -6249,7 +6303,7 @@
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
     </row>
-    <row r="7" spans="1:24" ht="80" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="112.5">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -6313,7 +6367,7 @@
       <c r="W7" s="21"/>
       <c r="X7" s="21"/>
     </row>
-    <row r="8" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="112.5">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -6377,7 +6431,7 @@
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
     </row>
-    <row r="9" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="112.5">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -6441,7 +6495,7 @@
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
     </row>
-    <row r="10" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="112.5">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -6505,7 +6559,7 @@
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
     </row>
-    <row r="11" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="112.5">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -6569,7 +6623,7 @@
       <c r="W11" s="21"/>
       <c r="X11" s="21"/>
     </row>
-    <row r="12" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="112.5">
       <c r="A12" s="23" t="s">
         <v>850</v>
       </c>
@@ -6639,7 +6693,7 @@
       <c r="W12" s="21"/>
       <c r="X12" s="21"/>
     </row>
-    <row r="13" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="112.5">
       <c r="A13" s="23" t="s">
         <v>849</v>
       </c>
@@ -6709,7 +6763,7 @@
       <c r="W13" s="21"/>
       <c r="X13" s="21"/>
     </row>
-    <row r="14" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="112.5">
       <c r="A14" s="23" t="s">
         <v>848</v>
       </c>
@@ -6779,7 +6833,7 @@
       <c r="W14" s="21"/>
       <c r="X14" s="21"/>
     </row>
-    <row r="15" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="112.5">
       <c r="A15" s="23" t="s">
         <v>847</v>
       </c>
@@ -6849,7 +6903,7 @@
       <c r="W15" s="21"/>
       <c r="X15" s="21"/>
     </row>
-    <row r="16" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="112.5">
       <c r="A16" s="23" t="s">
         <v>846</v>
       </c>
@@ -6919,7 +6973,7 @@
       <c r="W16" s="21"/>
       <c r="X16" s="21"/>
     </row>
-    <row r="17" spans="1:24" ht="80" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="112.5">
       <c r="A17" s="23" t="s">
         <v>845</v>
       </c>
@@ -6989,7 +7043,7 @@
       <c r="W17" s="21"/>
       <c r="X17" s="21"/>
     </row>
-    <row r="18" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="112.5">
       <c r="A18" s="23" t="s">
         <v>844</v>
       </c>
@@ -7059,7 +7113,7 @@
       <c r="W18" s="21"/>
       <c r="X18" s="21"/>
     </row>
-    <row r="19" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="112.5">
       <c r="A19" s="23" t="s">
         <v>843</v>
       </c>
@@ -7129,7 +7183,7 @@
       <c r="W19" s="21"/>
       <c r="X19" s="21"/>
     </row>
-    <row r="20" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="112.5">
       <c r="A20" s="23" t="s">
         <v>842</v>
       </c>
@@ -7199,7 +7253,7 @@
       <c r="W20" s="21"/>
       <c r="X20" s="21"/>
     </row>
-    <row r="21" spans="1:24" ht="100" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="112.5">
       <c r="A21" s="23" t="s">
         <v>841</v>
       </c>
@@ -7269,7 +7323,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="21"/>
     </row>
-    <row r="22" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="18.75">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -7295,7 +7349,7 @@
       <c r="W22" s="21"/>
       <c r="X22" s="21"/>
     </row>
-    <row r="23" spans="1:24" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="18.75">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -7330,26 +7384,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026BCBCE-4CBD-7246-9A76-5F67393CE992}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="19" customWidth="1"/>
-    <col min="8" max="9" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="19" customWidth="1"/>
+    <col min="8" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1"/>
-    <col min="12" max="12" width="56.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -7381,7 +7435,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>266</v>
       </c>
@@ -7413,7 +7467,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -7423,7 +7477,7 @@
       <c r="G3" s="27"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="1" t="s">
         <v>241</v>
       </c>
@@ -7461,7 +7515,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>271</v>
       </c>
@@ -7499,7 +7553,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
         <v>272</v>
       </c>
@@ -7537,7 +7591,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -7569,7 +7623,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>276</v>
       </c>
@@ -7601,7 +7655,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -7611,7 +7665,7 @@
       <c r="G12" s="27"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
         <v>241</v>
       </c>
@@ -7649,7 +7703,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="4" t="s">
         <v>271</v>
       </c>
@@ -7687,7 +7741,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="4" t="s">
         <v>272</v>
       </c>
@@ -7725,7 +7779,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -7757,7 +7811,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
         <v>277</v>
       </c>
@@ -7789,7 +7843,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -7799,7 +7853,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" s="1" t="s">
         <v>241</v>
       </c>
@@ -7837,7 +7891,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="4" t="s">
         <v>271</v>
       </c>
@@ -7875,7 +7929,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="4" t="s">
         <v>272</v>
       </c>
@@ -7913,7 +7967,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -7945,7 +7999,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
         <v>278</v>
       </c>
@@ -7977,7 +8031,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -7987,7 +8041,7 @@
       <c r="G30" s="27"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="30">
       <c r="A31" s="1" t="s">
         <v>241</v>
       </c>
@@ -8025,7 +8079,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="4" t="s">
         <v>271</v>
       </c>
@@ -8063,7 +8117,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="4" t="s">
         <v>272</v>
       </c>
@@ -8101,7 +8155,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="6" t="s">
         <v>10</v>
       </c>
@@ -8135,7 +8189,7 @@
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="9" t="s">
         <v>279</v>
       </c>
@@ -8169,7 +8223,7 @@
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -8183,7 +8237,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="30">
       <c r="A40" s="6" t="s">
         <v>241</v>
       </c>
@@ -8221,7 +8275,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="13" t="s">
         <v>271</v>
       </c>
@@ -8259,7 +8313,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="13" t="s">
         <v>272</v>
       </c>
@@ -8297,7 +8351,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="6" t="s">
         <v>10</v>
       </c>
@@ -8331,7 +8385,7 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="9" t="s">
         <v>280</v>
       </c>
@@ -8365,7 +8419,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -8379,7 +8433,7 @@
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
     </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="30">
       <c r="A49" s="6" t="s">
         <v>241</v>
       </c>
@@ -8417,7 +8471,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50" s="13" t="s">
         <v>271</v>
       </c>
@@ -8455,7 +8509,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" s="13" t="s">
         <v>272</v>
       </c>
@@ -8493,7 +8547,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="A55" s="6" t="s">
         <v>10</v>
       </c>
@@ -8527,7 +8581,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" s="9" t="s">
         <v>281</v>
       </c>
@@ -8561,7 +8615,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -8575,7 +8629,7 @@
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="30">
       <c r="A58" s="6" t="s">
         <v>241</v>
       </c>
@@ -8613,7 +8667,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12">
       <c r="A59" s="13" t="s">
         <v>271</v>
       </c>
@@ -8651,7 +8705,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" s="13" t="s">
         <v>272</v>
       </c>
@@ -8689,7 +8743,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12">
       <c r="A64" s="6" t="s">
         <v>10</v>
       </c>
@@ -8723,7 +8777,7 @@
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
     </row>
-    <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12">
       <c r="A65" s="9" t="s">
         <v>282</v>
       </c>
@@ -8757,7 +8811,7 @@
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -8771,7 +8825,7 @@
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
     </row>
-    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="30">
       <c r="A67" s="6" t="s">
         <v>241</v>
       </c>
@@ -8809,7 +8863,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12">
       <c r="A68" s="13" t="s">
         <v>271</v>
       </c>
@@ -8847,7 +8901,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12">
       <c r="A69" s="13" t="s">
         <v>272</v>
       </c>
@@ -8892,26 +8946,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAF93FA-38E5-45F4-AB60-57ED3B3EDFB0}">
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -8934,7 +8988,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -8957,7 +9011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -8986,7 +9040,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -9015,7 +9069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -9044,7 +9098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -9073,7 +9127,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
@@ -9102,7 +9156,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -9131,7 +9185,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -9160,7 +9214,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -9189,7 +9243,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -9218,7 +9272,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
@@ -9247,7 +9301,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -9270,7 +9324,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="3" t="s">
         <v>228</v>
       </c>
@@ -9293,7 +9347,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -9322,7 +9376,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -9351,7 +9405,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -9380,7 +9434,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -9409,7 +9463,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
@@ -9438,7 +9492,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
@@ -9467,7 +9521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="30">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -9496,7 +9550,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="30">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -9525,7 +9579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
@@ -9554,7 +9608,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -9583,7 +9637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
@@ -9612,7 +9666,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -9641,7 +9695,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -9664,7 +9718,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -9687,7 +9741,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -9716,7 +9770,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
@@ -9745,7 +9799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
@@ -9774,7 +9828,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="4" t="s">
         <v>33</v>
       </c>
@@ -9803,7 +9857,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
@@ -9832,7 +9886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -9861,7 +9915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="4" t="s">
         <v>38</v>
       </c>
@@ -9890,7 +9944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="30">
       <c r="A45" s="4" t="s">
         <v>38</v>
       </c>
@@ -9919,7 +9973,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -9948,7 +10002,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
@@ -9977,7 +10031,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="4" t="s">
         <v>41</v>
       </c>
@@ -10006,7 +10060,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
@@ -10035,7 +10089,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -10058,7 +10112,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -10081,7 +10135,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
@@ -10110,7 +10164,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="4" t="s">
         <v>33</v>
       </c>
@@ -10139,7 +10193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="4" t="s">
         <v>33</v>
       </c>
@@ -10168,7 +10222,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9">
       <c r="A59" s="4" t="s">
         <v>33</v>
       </c>
@@ -10197,7 +10251,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9">
       <c r="A60" s="4" t="s">
         <v>41</v>
       </c>
@@ -10226,7 +10280,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9">
       <c r="A61" s="4" t="s">
         <v>41</v>
       </c>
@@ -10255,7 +10309,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="30">
       <c r="A62" s="4" t="s">
         <v>38</v>
       </c>
@@ -10284,7 +10338,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="30">
       <c r="A63" s="4" t="s">
         <v>38</v>
       </c>
@@ -10313,7 +10367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9">
       <c r="A64" s="4" t="s">
         <v>48</v>
       </c>
@@ -10342,7 +10396,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9">
       <c r="A65" s="4" t="s">
         <v>48</v>
       </c>
@@ -10371,7 +10425,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9">
       <c r="A66" s="4" t="s">
         <v>41</v>
       </c>
@@ -10400,7 +10454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9">
       <c r="A67" s="4" t="s">
         <v>41</v>
       </c>
@@ -10429,7 +10483,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -10452,7 +10506,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="3" t="s">
         <v>8</v>
       </c>
@@ -10475,7 +10529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
         <v>15</v>
       </c>
@@ -10504,7 +10558,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9">
       <c r="A75" s="4" t="s">
         <v>33</v>
       </c>
@@ -10533,7 +10587,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="A76" s="4" t="s">
         <v>33</v>
       </c>
@@ -10562,7 +10616,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9">
       <c r="A77" s="4" t="s">
         <v>33</v>
       </c>
@@ -10591,7 +10645,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9">
       <c r="A78" s="4" t="s">
         <v>41</v>
       </c>
@@ -10620,7 +10674,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9">
       <c r="A79" s="4" t="s">
         <v>41</v>
       </c>
@@ -10649,7 +10703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="15.95" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>42</v>
       </c>
@@ -10678,7 +10732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="15.95" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>42</v>
       </c>
@@ -10707,7 +10761,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
@@ -10730,7 +10784,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="30">
       <c r="A86" s="3" t="s">
         <v>229</v>
       </c>
@@ -10753,7 +10807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
         <v>15</v>
       </c>
@@ -10782,7 +10836,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9">
       <c r="A89" s="4" t="s">
         <v>33</v>
       </c>
@@ -10811,7 +10865,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9">
       <c r="A90" s="4" t="s">
         <v>33</v>
       </c>
@@ -10840,7 +10894,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9">
       <c r="A91" s="4" t="s">
         <v>33</v>
       </c>
@@ -10869,7 +10923,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9">
       <c r="A92" s="4" t="s">
         <v>36</v>
       </c>
@@ -10898,7 +10952,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9">
       <c r="A93" s="4" t="s">
         <v>36</v>
       </c>
@@ -10927,7 +10981,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="15.95" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>38</v>
       </c>
@@ -10956,7 +11010,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="15.95" customHeight="1">
       <c r="A95" s="4" t="s">
         <v>38</v>
       </c>
@@ -10985,7 +11039,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9">
       <c r="A99" s="1" t="s">
         <v>10</v>
       </c>
@@ -11008,7 +11062,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="15.95" customHeight="1">
       <c r="A100" s="3" t="s">
         <v>9</v>
       </c>
@@ -11031,7 +11085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9">
       <c r="A102" s="1" t="s">
         <v>15</v>
       </c>
@@ -11060,7 +11114,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9">
       <c r="A103" s="4" t="s">
         <v>33</v>
       </c>
@@ -11087,7 +11141,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9">
       <c r="A104" s="4" t="s">
         <v>33</v>
       </c>
@@ -11116,7 +11170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9">
       <c r="A105" s="4" t="s">
         <v>33</v>
       </c>
@@ -11145,7 +11199,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9">
       <c r="A106" s="4" t="s">
         <v>32</v>
       </c>
@@ -11174,7 +11228,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9">
       <c r="A107" s="4" t="s">
         <v>33</v>
       </c>
@@ -11203,7 +11257,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9">
       <c r="A108" s="4" t="s">
         <v>33</v>
       </c>
@@ -11232,7 +11286,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9">
       <c r="A109" s="4" t="s">
         <v>33</v>
       </c>
@@ -11261,7 +11315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9">
       <c r="A110" s="4" t="s">
         <v>33</v>
       </c>
@@ -11290,7 +11344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9">
       <c r="A114" s="1" t="s">
         <v>10</v>
       </c>
@@ -11313,7 +11367,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="15.95" customHeight="1">
       <c r="A115" s="3" t="s">
         <v>21</v>
       </c>
@@ -11336,7 +11390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9">
       <c r="A117" s="1" t="s">
         <v>15</v>
       </c>
@@ -11365,7 +11419,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9">
       <c r="A118" s="4" t="s">
         <v>33</v>
       </c>
@@ -11392,7 +11446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9">
       <c r="A119" s="4" t="s">
         <v>33</v>
       </c>
@@ -11421,7 +11475,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9">
       <c r="A120" s="4" t="s">
         <v>33</v>
       </c>
@@ -11450,7 +11504,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9">
       <c r="A121" s="4" t="s">
         <v>32</v>
       </c>
@@ -11479,7 +11533,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9">
       <c r="A122" s="4" t="s">
         <v>33</v>
       </c>
@@ -11508,7 +11562,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9">
       <c r="A123" s="4" t="s">
         <v>33</v>
       </c>
@@ -11537,7 +11591,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9">
       <c r="A124" s="4" t="s">
         <v>33</v>
       </c>
@@ -11566,7 +11620,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9">
       <c r="A125" s="4" t="s">
         <v>33</v>
       </c>
@@ -11595,7 +11649,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -11618,7 +11672,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="15.95" customHeight="1">
       <c r="A130" s="3" t="s">
         <v>22</v>
       </c>
@@ -11641,7 +11695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9">
       <c r="A132" s="1" t="s">
         <v>15</v>
       </c>
@@ -11670,7 +11724,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9">
       <c r="A133" s="4" t="s">
         <v>33</v>
       </c>
@@ -11697,7 +11751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9">
       <c r="A134" s="4" t="s">
         <v>33</v>
       </c>
@@ -11726,7 +11780,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9">
       <c r="A135" s="4" t="s">
         <v>33</v>
       </c>
@@ -11755,7 +11809,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9">
       <c r="A136" s="4" t="s">
         <v>32</v>
       </c>
@@ -11784,7 +11838,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9">
       <c r="A137" s="4" t="s">
         <v>33</v>
       </c>
@@ -11813,7 +11867,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9">
       <c r="A138" s="4" t="s">
         <v>33</v>
       </c>
@@ -11842,7 +11896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9">
       <c r="A139" s="4" t="s">
         <v>33</v>
       </c>
@@ -11871,7 +11925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9">
       <c r="A140" s="4" t="s">
         <v>33</v>
       </c>
@@ -11900,7 +11954,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9">
       <c r="A144" s="1" t="s">
         <v>10</v>
       </c>
@@ -11923,7 +11977,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" ht="15.95" customHeight="1">
       <c r="A145" s="3" t="s">
         <v>23</v>
       </c>
@@ -11946,7 +12000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9">
       <c r="A147" s="1" t="s">
         <v>15</v>
       </c>
@@ -11975,7 +12029,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" ht="15.95" customHeight="1">
       <c r="A148" s="4" t="s">
         <v>33</v>
       </c>
@@ -12002,7 +12056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" ht="15.95" customHeight="1">
       <c r="A149" s="4" t="s">
         <v>33</v>
       </c>
@@ -12031,7 +12085,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" ht="15.95" customHeight="1">
       <c r="A150" s="4" t="s">
         <v>33</v>
       </c>
@@ -12060,7 +12114,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" ht="15.95" customHeight="1">
       <c r="A151" s="4" t="s">
         <v>32</v>
       </c>
@@ -12089,7 +12143,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" ht="15.95" customHeight="1">
       <c r="A152" s="4" t="s">
         <v>33</v>
       </c>
@@ -12118,7 +12172,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" ht="15.95" customHeight="1">
       <c r="A153" s="4" t="s">
         <v>33</v>
       </c>
@@ -12147,7 +12201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" ht="15.95" customHeight="1">
       <c r="A154" s="4" t="s">
         <v>33</v>
       </c>
@@ -12176,7 +12230,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" ht="15.95" customHeight="1">
       <c r="A155" s="4" t="s">
         <v>33</v>
       </c>
@@ -12203,6 +12257,197 @@
       </c>
       <c r="I155" s="3" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A160" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="D160" s="4">
+        <v>4</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="F160" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="G160" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A163" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E163" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H163" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I163" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A164" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E164" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A165" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>886</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E165" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>888</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="15.95" customHeight="1">
+      <c r="A166" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E166" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -12222,20 +12467,20 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -12258,7 +12503,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="3" t="s">
         <v>156</v>
       </c>
@@ -12281,7 +12526,7 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -12310,7 +12555,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -12337,7 +12582,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -12366,7 +12611,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -12395,7 +12640,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -12424,7 +12669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>

</xml_diff>